<commit_message>
update ExcelReader and ExcelWriter
</commit_message>
<xml_diff>
--- a/SiteTemplate/WebSite/Content/ReportTemplate/测试模板.xlsx
+++ b/SiteTemplate/WebSite/Content/ReportTemplate/测试模板.xlsx
@@ -28,31 +28,10 @@
             <sz val="9"/>
             <color auto="1"/>
             <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
+            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">数据格式错误
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color auto="1"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>必须是GUI</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="宋体"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">D
+必须是GUID
 </t>
         </r>
       </text>
@@ -980,7 +959,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1034,6 +1013,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color auto="1"/>
+      <name val="宋体"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1084,7 +1070,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" numFmtId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fontId="0" numFmtId="0" fillId="0" borderId="0" xfId="0"/>
     <xf applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="3" numFmtId="0" fillId="2" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1106,6 +1092,9 @@
     </xf>
     <xf applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" fontId="4" numFmtId="0" fillId="3" borderId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyBorder="1" applyAlignment="1" fontId="0" numFmtId="0" fillId="0" borderId="2" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3472,7 +3461,7 @@
       </c>
     </row>
     <row r="3" s="2" customFormat="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">

</xml_diff>